<commit_message>
* Improved the work efficient scan implementation only enqueuing relevant work items. Speedup of 3! * Finished chapter about work efficient scan
</commit_message>
<xml_diff>
--- a/latex/charts/2013_08_01_scan_thesis.xlsx
+++ b/latex/charts/2013_08_01_scan_thesis.xlsx
@@ -1160,82 +1160,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2.5300000000000001E-3</c:v>
+                  <c:v>2.562E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3550000000000001E-3</c:v>
+                  <c:v>7.5199999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.6800000000000004E-4</c:v>
+                  <c:v>1.3829999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8600000000000004E-4</c:v>
+                  <c:v>1.116E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.792E-3</c:v>
+                  <c:v>2.006E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3680000000000001E-3</c:v>
+                  <c:v>1.918E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4200000000000004E-4</c:v>
+                  <c:v>2.1559999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5200000000000002E-4</c:v>
+                  <c:v>1.2589999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.946E-3</c:v>
+                  <c:v>2.3700000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.732E-3</c:v>
+                  <c:v>1.6869999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.1000000000000002E-4</c:v>
+                  <c:v>2.604E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.6999999999999996E-4</c:v>
+                  <c:v>3.0699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5920000000000001E-3</c:v>
+                  <c:v>2.4260000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.941E-3</c:v>
+                  <c:v>2.3029999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5579999999999999E-3</c:v>
+                  <c:v>2.8449999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.699E-3</c:v>
+                  <c:v>2.6480000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.1790000000000004E-3</c:v>
+                  <c:v>3.192E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.672E-3</c:v>
+                  <c:v>4.3730000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5169999999999999E-2</c:v>
+                  <c:v>6.8950000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0158999999999998E-2</c:v>
+                  <c:v>1.1199000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.1520999999999996E-2</c:v>
+                  <c:v>1.9886999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.12579599999999999</c:v>
+                  <c:v>3.7275000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.25885999999999998</c:v>
+                  <c:v>7.8276999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.544825</c:v>
+                  <c:v>0.15335099999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.0735710000000001</c:v>
+                  <c:v>0.30188100000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2140529999999998</c:v>
+                  <c:v>0.60310699999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,11 +1636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94048192"/>
-        <c:axId val="94048768"/>
+        <c:axId val="67473344"/>
+        <c:axId val="67473920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94048192"/>
+        <c:axId val="67473344"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1671,12 +1671,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94048768"/>
+        <c:crossAx val="67473920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94048768"/>
+        <c:axId val="67473920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1707,7 +1707,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94048192"/>
+        <c:crossAx val="67473344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2066,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN17" sqref="AN17"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="M89" sqref="M89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,7 +3381,7 @@
         <v>8</v>
       </c>
       <c r="B66">
-        <v>9.0407000000000001E-2</v>
+        <v>7.5596999999999998E-2</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -3421,28 +3421,28 @@
         <v>2</v>
       </c>
       <c r="B68">
-        <v>1.9070000000000001E-3</v>
+        <v>1.3630000000000001E-3</v>
       </c>
       <c r="C68">
-        <v>1.9940000000000001E-3</v>
+        <v>1.668E-3</v>
       </c>
       <c r="D68">
-        <v>4.8099999999999998E-4</v>
+        <v>1.011E-3</v>
       </c>
       <c r="E68">
-        <v>4.73E-4</v>
+        <v>1.1199999999999999E-3</v>
       </c>
       <c r="F68">
-        <v>1.4300000000000001E-4</v>
+        <v>1.8900000000000001E-4</v>
       </c>
       <c r="G68">
-        <v>6.3E-5</v>
+        <v>1.25E-4</v>
       </c>
       <c r="H68">
         <v>256</v>
       </c>
       <c r="I68">
-        <v>2.5300000000000001E-3</v>
+        <v>2.562E-3</v>
       </c>
       <c r="J68" t="s">
         <v>7</v>
@@ -3453,28 +3453,28 @@
         <v>4</v>
       </c>
       <c r="B69">
-        <v>1.075E-3</v>
+        <v>3.5399999999999999E-4</v>
       </c>
       <c r="C69">
-        <v>1.3649999999999999E-3</v>
+        <v>3.2899999999999997E-4</v>
       </c>
       <c r="D69">
-        <v>1.7699999999999999E-4</v>
+        <v>2.7300000000000002E-4</v>
       </c>
       <c r="E69">
-        <v>3.4E-5</v>
+        <v>4.8999999999999998E-5</v>
       </c>
       <c r="F69">
-        <v>1.0399999999999999E-4</v>
+        <v>1.2400000000000001E-4</v>
       </c>
       <c r="G69">
-        <v>1.5E-5</v>
+        <v>1.9000000000000001E-5</v>
       </c>
       <c r="H69">
         <v>256</v>
       </c>
       <c r="I69">
-        <v>1.3550000000000001E-3</v>
+        <v>7.5199999999999996E-4</v>
       </c>
       <c r="J69" t="s">
         <v>7</v>
@@ -3485,28 +3485,28 @@
         <v>8</v>
       </c>
       <c r="B70">
-        <v>2.3000000000000001E-4</v>
+        <v>1.5899999999999999E-4</v>
       </c>
       <c r="C70">
-        <v>8.7999999999999998E-5</v>
+        <v>6.6000000000000005E-5</v>
       </c>
       <c r="D70">
-        <v>2.2599999999999999E-4</v>
+        <v>1.1039999999999999E-3</v>
       </c>
       <c r="E70">
-        <v>5.3000000000000001E-5</v>
+        <v>1.0889999999999999E-3</v>
       </c>
       <c r="F70">
-        <v>1.11E-4</v>
+        <v>1.2E-4</v>
       </c>
       <c r="G70">
-        <v>2.9E-5</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H70">
         <v>256</v>
       </c>
       <c r="I70">
-        <v>5.6800000000000004E-4</v>
+        <v>1.3829999999999999E-3</v>
       </c>
       <c r="J70" t="s">
         <v>7</v>
@@ -3517,28 +3517,28 @@
         <v>16</v>
       </c>
       <c r="B71">
-        <v>2.6899999999999998E-4</v>
+        <v>6.6E-4</v>
       </c>
       <c r="C71">
-        <v>2.24E-4</v>
+        <v>7.6599999999999997E-4</v>
       </c>
       <c r="D71">
-        <v>2.1599999999999999E-4</v>
+        <v>3.3500000000000001E-4</v>
       </c>
       <c r="E71">
-        <v>2.0000000000000002E-5</v>
+        <v>2.8E-5</v>
       </c>
       <c r="F71">
-        <v>1E-4</v>
+        <v>1.22E-4</v>
       </c>
       <c r="G71">
-        <v>1.2999999999999999E-5</v>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="H71">
         <v>256</v>
       </c>
       <c r="I71">
-        <v>5.8600000000000004E-4</v>
+        <v>1.116E-3</v>
       </c>
       <c r="J71" t="s">
         <v>7</v>
@@ -3549,28 +3549,28 @@
         <v>32</v>
       </c>
       <c r="B72">
-        <v>2.5300000000000002E-4</v>
+        <v>2.2499999999999999E-4</v>
       </c>
       <c r="C72">
-        <v>1.9100000000000001E-4</v>
+        <v>5.7000000000000003E-5</v>
       </c>
       <c r="D72">
-        <v>1.4289999999999999E-3</v>
+        <v>1.5579999999999999E-3</v>
       </c>
       <c r="E72">
-        <v>1.616E-3</v>
+        <v>1.5529999999999999E-3</v>
       </c>
       <c r="F72">
-        <v>1.1E-4</v>
+        <v>2.24E-4</v>
       </c>
       <c r="G72">
-        <v>1.2999999999999999E-5</v>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="H72">
         <v>256</v>
       </c>
       <c r="I72">
-        <v>1.792E-3</v>
+        <v>2.006E-3</v>
       </c>
       <c r="J72" t="s">
         <v>7</v>
@@ -3581,28 +3581,28 @@
         <v>64</v>
       </c>
       <c r="B73">
-        <v>9.990000000000001E-4</v>
+        <v>3.2699999999999998E-4</v>
       </c>
       <c r="C73">
-        <v>1.258E-3</v>
+        <v>1.63E-4</v>
       </c>
       <c r="D73">
-        <v>2.6400000000000002E-4</v>
+        <v>1.2409999999999999E-3</v>
       </c>
       <c r="E73">
-        <v>2.8E-5</v>
+        <v>5.5800000000000001E-4</v>
       </c>
       <c r="F73">
-        <v>1.05E-4</v>
+        <v>3.5100000000000002E-4</v>
       </c>
       <c r="G73">
-        <v>1.7E-5</v>
+        <v>7.4999999999999993E-5</v>
       </c>
       <c r="H73">
         <v>256</v>
       </c>
       <c r="I73">
-        <v>1.3680000000000001E-3</v>
+        <v>1.918E-3</v>
       </c>
       <c r="J73" t="s">
         <v>7</v>
@@ -3613,28 +3613,28 @@
         <v>128</v>
       </c>
       <c r="B74">
-        <v>3.2499999999999999E-4</v>
+        <v>1.132E-3</v>
       </c>
       <c r="C74">
-        <v>2.7E-4</v>
+        <v>1.0579999999999999E-3</v>
       </c>
       <c r="D74">
-        <v>2.9399999999999999E-4</v>
+        <v>6.8199999999999999E-4</v>
       </c>
       <c r="E74">
-        <v>2.5999999999999998E-5</v>
+        <v>1.3799999999999999E-4</v>
       </c>
       <c r="F74">
-        <v>1.2300000000000001E-4</v>
+        <v>3.4200000000000002E-4</v>
       </c>
       <c r="G74">
-        <v>1.5E-5</v>
+        <v>1.56E-4</v>
       </c>
       <c r="H74">
         <v>256</v>
       </c>
       <c r="I74">
-        <v>7.4200000000000004E-4</v>
+        <v>2.1559999999999999E-3</v>
       </c>
       <c r="J74" t="s">
         <v>7</v>
@@ -3645,28 +3645,28 @@
         <v>256</v>
       </c>
       <c r="B75">
-        <v>2.3800000000000001E-4</v>
+        <v>5.5400000000000002E-4</v>
       </c>
       <c r="C75">
-        <v>1.8100000000000001E-4</v>
+        <v>5.31E-4</v>
       </c>
       <c r="D75">
-        <v>3.1199999999999999E-4</v>
+        <v>5.2899999999999996E-4</v>
       </c>
       <c r="E75">
-        <v>2.3E-5</v>
+        <v>4.6E-5</v>
       </c>
       <c r="F75">
-        <v>1.03E-4</v>
+        <v>1.76E-4</v>
       </c>
       <c r="G75">
-        <v>1.1E-5</v>
+        <v>2.4000000000000001E-5</v>
       </c>
       <c r="H75">
         <v>256</v>
       </c>
       <c r="I75">
-        <v>6.5200000000000002E-4</v>
+        <v>1.2589999999999999E-3</v>
       </c>
       <c r="J75" t="s">
         <v>7</v>
@@ -3677,28 +3677,28 @@
         <v>512</v>
       </c>
       <c r="B76">
-        <v>1.3519999999999999E-3</v>
+        <v>1.111E-3</v>
       </c>
       <c r="C76">
-        <v>1.7240000000000001E-3</v>
+        <v>9.3400000000000004E-4</v>
       </c>
       <c r="D76">
-        <v>4.6900000000000002E-4</v>
+        <v>8.7399999999999999E-4</v>
       </c>
       <c r="E76">
-        <v>2.0000000000000001E-4</v>
+        <v>1.5699999999999999E-4</v>
       </c>
       <c r="F76">
-        <v>1.26E-4</v>
+        <v>3.8499999999999998E-4</v>
       </c>
       <c r="G76">
-        <v>1.4E-5</v>
+        <v>1.66E-4</v>
       </c>
       <c r="H76">
         <v>256</v>
       </c>
       <c r="I76">
-        <v>1.946E-3</v>
+        <v>2.3700000000000001E-3</v>
       </c>
       <c r="J76" t="s">
         <v>7</v>
@@ -3709,28 +3709,28 @@
         <v>1024</v>
       </c>
       <c r="B77">
-        <v>9.2299999999999999E-4</v>
+        <v>6.4000000000000005E-4</v>
       </c>
       <c r="C77">
-        <v>1.1410000000000001E-3</v>
+        <v>3.8499999999999998E-4</v>
       </c>
       <c r="D77">
-        <v>7.0399999999999998E-4</v>
+        <v>7.54E-4</v>
       </c>
       <c r="E77">
-        <v>5.0500000000000002E-4</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="F77">
-        <v>1.05E-4</v>
+        <v>2.92E-4</v>
       </c>
       <c r="G77">
-        <v>1.2999999999999999E-5</v>
+        <v>2.6999999999999999E-5</v>
       </c>
       <c r="H77">
         <v>256</v>
       </c>
       <c r="I77">
-        <v>1.732E-3</v>
+        <v>1.6869999999999999E-3</v>
       </c>
       <c r="J77" t="s">
         <v>7</v>
@@ -3741,28 +3741,28 @@
         <v>2048</v>
       </c>
       <c r="B78">
-        <v>2.4800000000000001E-4</v>
+        <v>1.405E-3</v>
       </c>
       <c r="C78">
-        <v>1.8599999999999999E-4</v>
+        <v>1.408E-3</v>
       </c>
       <c r="D78">
-        <v>3.5799999999999997E-4</v>
+        <v>8.1599999999999999E-4</v>
       </c>
       <c r="E78">
-        <v>2.0999999999999999E-5</v>
+        <v>1.36E-4</v>
       </c>
       <c r="F78">
-        <v>1.05E-4</v>
+        <v>3.8200000000000002E-4</v>
       </c>
       <c r="G78">
-        <v>1.2E-5</v>
+        <v>1.5799999999999999E-4</v>
       </c>
       <c r="H78">
         <v>256</v>
       </c>
       <c r="I78">
-        <v>7.1000000000000002E-4</v>
+        <v>2.604E-3</v>
       </c>
       <c r="J78" t="s">
         <v>7</v>
@@ -3773,28 +3773,28 @@
         <v>4096</v>
       </c>
       <c r="B79">
-        <v>2.5399999999999999E-4</v>
+        <v>1.7290000000000001E-3</v>
       </c>
       <c r="C79">
-        <v>1.8200000000000001E-4</v>
+        <v>1.8749999999999999E-3</v>
       </c>
       <c r="D79">
-        <v>4.0499999999999998E-4</v>
+        <v>9.7799999999999992E-4</v>
       </c>
       <c r="E79">
-        <v>2.5000000000000001E-5</v>
+        <v>1.8599999999999999E-4</v>
       </c>
       <c r="F79">
-        <v>1.11E-4</v>
+        <v>3.6299999999999999E-4</v>
       </c>
       <c r="G79">
-        <v>1.2E-5</v>
+        <v>1.3999999999999999E-4</v>
       </c>
       <c r="H79">
         <v>256</v>
       </c>
       <c r="I79">
-        <v>7.6999999999999996E-4</v>
+        <v>3.0699999999999998E-3</v>
       </c>
       <c r="J79" t="s">
         <v>7</v>
@@ -3805,28 +3805,28 @@
         <v>8192</v>
       </c>
       <c r="B80">
-        <v>6.9300000000000004E-4</v>
+        <v>9.2100000000000005E-4</v>
       </c>
       <c r="C80">
-        <v>7.5299999999999998E-4</v>
+        <v>6.0300000000000002E-4</v>
       </c>
       <c r="D80">
-        <v>7.4799999999999997E-4</v>
+        <v>1.16E-3</v>
       </c>
       <c r="E80">
-        <v>8.0000000000000007E-5</v>
+        <v>2.2599999999999999E-4</v>
       </c>
       <c r="F80">
-        <v>1.5200000000000001E-4</v>
+        <v>3.4499999999999998E-4</v>
       </c>
       <c r="G80">
-        <v>1.7E-5</v>
+        <v>4.6E-5</v>
       </c>
       <c r="H80">
         <v>256</v>
       </c>
       <c r="I80">
-        <v>1.5920000000000001E-3</v>
+        <v>2.4260000000000002E-3</v>
       </c>
       <c r="J80" t="s">
         <v>7</v>
@@ -3837,28 +3837,28 @@
         <v>16384</v>
       </c>
       <c r="B81">
-        <v>1.1509999999999999E-3</v>
+        <v>4.8099999999999998E-4</v>
       </c>
       <c r="C81">
-        <v>1.3760000000000001E-3</v>
+        <v>2.99E-4</v>
       </c>
       <c r="D81">
-        <v>5.9999999999999995E-4</v>
+        <v>1.4319999999999999E-3</v>
       </c>
       <c r="E81">
-        <v>3.0000000000000001E-5</v>
+        <v>6.4199999999999999E-4</v>
       </c>
       <c r="F81">
-        <v>1.9100000000000001E-4</v>
+        <v>3.8999999999999999E-4</v>
       </c>
       <c r="G81">
-        <v>5.8E-5</v>
+        <v>1.6899999999999999E-4</v>
       </c>
       <c r="H81">
         <v>256</v>
       </c>
       <c r="I81">
-        <v>1.941E-3</v>
+        <v>2.3029999999999999E-3</v>
       </c>
       <c r="J81" t="s">
         <v>7</v>
@@ -3869,28 +3869,28 @@
         <v>32768</v>
       </c>
       <c r="B82">
-        <v>3.3399999999999999E-4</v>
+        <v>1.17E-3</v>
       </c>
       <c r="C82">
-        <v>1.7200000000000001E-4</v>
+        <v>1.067E-3</v>
       </c>
       <c r="D82">
-        <v>9.990000000000001E-4</v>
+        <v>1.217E-3</v>
       </c>
       <c r="E82">
-        <v>7.7999999999999999E-5</v>
+        <v>2.9700000000000001E-4</v>
       </c>
       <c r="F82">
-        <v>2.2499999999999999E-4</v>
+        <v>4.5800000000000002E-4</v>
       </c>
       <c r="G82">
-        <v>7.7999999999999999E-5</v>
+        <v>1E-4</v>
       </c>
       <c r="H82">
         <v>256</v>
       </c>
       <c r="I82">
-        <v>1.5579999999999999E-3</v>
+        <v>2.8449999999999999E-3</v>
       </c>
       <c r="J82" t="s">
         <v>7</v>
@@ -3901,28 +3901,28 @@
         <v>65536</v>
       </c>
       <c r="B83">
-        <v>4.6900000000000002E-4</v>
+        <v>6.9200000000000002E-4</v>
       </c>
       <c r="C83">
-        <v>1.8200000000000001E-4</v>
+        <v>2.0799999999999999E-4</v>
       </c>
       <c r="D83">
-        <v>1.8309999999999999E-3</v>
+        <v>1.3619999999999999E-3</v>
       </c>
       <c r="E83">
-        <v>1.6699999999999999E-4</v>
+        <v>1.16E-4</v>
       </c>
       <c r="F83">
-        <v>3.9899999999999999E-4</v>
+        <v>5.9400000000000002E-4</v>
       </c>
       <c r="G83">
-        <v>1.2899999999999999E-4</v>
+        <v>1.5799999999999999E-4</v>
       </c>
       <c r="H83">
         <v>256</v>
       </c>
       <c r="I83">
-        <v>2.699E-3</v>
+        <v>2.6480000000000002E-3</v>
       </c>
       <c r="J83" t="s">
         <v>7</v>
@@ -3933,28 +3933,28 @@
         <v>131072</v>
       </c>
       <c r="B84">
-        <v>5.9500000000000004E-4</v>
+        <v>8.5899999999999995E-4</v>
       </c>
       <c r="C84">
-        <v>1.73E-4</v>
+        <v>2.0900000000000001E-4</v>
       </c>
       <c r="D84">
-        <v>2.99E-3</v>
+        <v>1.622E-3</v>
       </c>
       <c r="E84">
-        <v>3.6999999999999998E-5</v>
+        <v>2.2900000000000001E-4</v>
       </c>
       <c r="F84">
-        <v>5.9500000000000004E-4</v>
+        <v>7.1000000000000002E-4</v>
       </c>
       <c r="G84">
-        <v>2.2000000000000001E-4</v>
+        <v>3.1000000000000001E-5</v>
       </c>
       <c r="H84">
         <v>256</v>
       </c>
       <c r="I84">
-        <v>4.1790000000000004E-3</v>
+        <v>3.192E-3</v>
       </c>
       <c r="J84" t="s">
         <v>7</v>
@@ -3965,28 +3965,28 @@
         <v>262144</v>
       </c>
       <c r="B85">
-        <v>8.7000000000000001E-4</v>
+        <v>1.2520000000000001E-3</v>
       </c>
       <c r="C85">
-        <v>1.85E-4</v>
+        <v>9.7E-5</v>
       </c>
       <c r="D85">
-        <v>5.849E-3</v>
+        <v>2.2030000000000001E-3</v>
       </c>
       <c r="E85">
-        <v>9.2E-5</v>
+        <v>1.0399999999999999E-4</v>
       </c>
       <c r="F85">
-        <v>9.5399999999999999E-4</v>
+        <v>9.1799999999999998E-4</v>
       </c>
       <c r="G85">
-        <v>4.9600000000000002E-4</v>
+        <v>1.3300000000000001E-4</v>
       </c>
       <c r="H85">
         <v>256</v>
       </c>
       <c r="I85">
-        <v>7.672E-3</v>
+        <v>4.3730000000000002E-3</v>
       </c>
       <c r="J85" t="s">
         <v>7</v>
@@ -3997,28 +3997,28 @@
         <v>524288</v>
       </c>
       <c r="B86">
-        <v>1.4649999999999999E-3</v>
+        <v>1.668E-3</v>
       </c>
       <c r="C86">
-        <v>1.9100000000000001E-4</v>
+        <v>6.6000000000000005E-5</v>
       </c>
       <c r="D86">
-        <v>1.1742000000000001E-2</v>
+        <v>3.6449999999999998E-3</v>
       </c>
       <c r="E86">
-        <v>1.02E-4</v>
+        <v>9.7E-5</v>
       </c>
       <c r="F86">
-        <v>1.9629999999999999E-3</v>
+        <v>1.5820000000000001E-3</v>
       </c>
       <c r="G86">
-        <v>1.271E-3</v>
+        <v>4.6099999999999998E-4</v>
       </c>
       <c r="H86">
         <v>256</v>
       </c>
       <c r="I86">
-        <v>1.5169999999999999E-2</v>
+        <v>6.8950000000000001E-3</v>
       </c>
       <c r="J86" t="s">
         <v>7</v>
@@ -4029,28 +4029,28 @@
         <v>1048576</v>
       </c>
       <c r="B87">
-        <v>2.65E-3</v>
+        <v>2.7499999999999998E-3</v>
       </c>
       <c r="C87">
-        <v>3.0400000000000002E-4</v>
+        <v>2.52E-4</v>
       </c>
       <c r="D87">
-        <v>2.3875E-2</v>
+        <v>5.9800000000000001E-3</v>
       </c>
       <c r="E87">
-        <v>9.5000000000000005E-5</v>
+        <v>9.0000000000000006E-5</v>
       </c>
       <c r="F87">
-        <v>3.6340000000000001E-3</v>
+        <v>2.4689999999999998E-3</v>
       </c>
       <c r="G87">
-        <v>2.2859999999999998E-3</v>
+        <v>3.3100000000000002E-4</v>
       </c>
       <c r="H87">
         <v>256</v>
       </c>
       <c r="I87">
-        <v>3.0158999999999998E-2</v>
+        <v>1.1199000000000001E-2</v>
       </c>
       <c r="J87" t="s">
         <v>7</v>
@@ -4061,28 +4061,28 @@
         <v>2097152</v>
       </c>
       <c r="B88">
-        <v>5.6940000000000003E-3</v>
+        <v>4.6940000000000003E-3</v>
       </c>
       <c r="C88">
-        <v>1.4599999999999999E-3</v>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="D88">
-        <v>5.0599999999999999E-2</v>
+        <v>1.0940999999999999E-2</v>
       </c>
       <c r="E88">
-        <v>1.3439999999999999E-3</v>
+        <v>1.4899999999999999E-4</v>
       </c>
       <c r="F88">
-        <v>2.5225999999999998E-2</v>
+        <v>4.2529999999999998E-3</v>
       </c>
       <c r="G88">
-        <v>2.9281999999999999E-2</v>
+        <v>6.1700000000000004E-4</v>
       </c>
       <c r="H88">
         <v>256</v>
       </c>
       <c r="I88">
-        <v>8.1520999999999996E-2</v>
+        <v>1.9886999999999998E-2</v>
       </c>
       <c r="J88" t="s">
         <v>7</v>
@@ -4093,28 +4093,28 @@
         <v>4194304</v>
       </c>
       <c r="B89">
-        <v>8.6189999999999999E-3</v>
+        <v>8.4480000000000006E-3</v>
       </c>
       <c r="C89">
-        <v>1.209E-3</v>
+        <v>5.9900000000000003E-4</v>
       </c>
       <c r="D89">
-        <v>0.102836</v>
+        <v>2.1006E-2</v>
       </c>
       <c r="E89">
-        <v>1.8599999999999999E-4</v>
+        <v>1.11E-4</v>
       </c>
       <c r="F89">
-        <v>1.434E-2</v>
+        <v>7.8209999999999998E-3</v>
       </c>
       <c r="G89">
-        <v>1.0283E-2</v>
+        <v>1.2099999999999999E-3</v>
       </c>
       <c r="H89">
         <v>256</v>
       </c>
       <c r="I89">
-        <v>0.12579599999999999</v>
+        <v>3.7275000000000003E-2</v>
       </c>
       <c r="J89" t="s">
         <v>7</v>
@@ -4125,28 +4125,28 @@
         <v>8388608</v>
       </c>
       <c r="B90">
-        <v>1.5566999999999999E-2</v>
+        <v>1.6354E-2</v>
       </c>
       <c r="C90">
-        <v>4.8000000000000001E-5</v>
+        <v>4.66E-4</v>
       </c>
       <c r="D90">
-        <v>0.21432100000000001</v>
+        <v>4.1776000000000001E-2</v>
       </c>
       <c r="E90">
-        <v>2.1000000000000001E-4</v>
+        <v>9.68E-4</v>
       </c>
       <c r="F90">
-        <v>2.8972000000000001E-2</v>
+        <v>2.0147999999999999E-2</v>
       </c>
       <c r="G90">
-        <v>2.1693E-2</v>
+        <v>4.4010000000000004E-3</v>
       </c>
       <c r="H90">
         <v>256</v>
       </c>
       <c r="I90">
-        <v>0.25885999999999998</v>
+        <v>7.8276999999999999E-2</v>
       </c>
       <c r="J90" t="s">
         <v>7</v>
@@ -4157,28 +4157,28 @@
         <v>16777216</v>
       </c>
       <c r="B91">
-        <v>4.1236000000000002E-2</v>
+        <v>3.6672000000000003E-2</v>
       </c>
       <c r="C91">
-        <v>8.4999999999999995E-4</v>
+        <v>2.1900000000000001E-4</v>
       </c>
       <c r="D91">
-        <v>0.44387799999999999</v>
+        <v>8.0421999999999993E-2</v>
       </c>
       <c r="E91">
-        <v>1.4339999999999999E-3</v>
+        <v>2.52E-4</v>
       </c>
       <c r="F91">
-        <v>5.9709999999999999E-2</v>
+        <v>3.6255999999999997E-2</v>
       </c>
       <c r="G91">
-        <v>3.9029000000000001E-2</v>
+        <v>5.4949999999999999E-3</v>
       </c>
       <c r="H91">
         <v>256</v>
       </c>
       <c r="I91">
-        <v>0.544825</v>
+        <v>0.15335099999999999</v>
       </c>
       <c r="J91" t="s">
         <v>7</v>
@@ -4189,28 +4189,28 @@
         <v>33554432</v>
       </c>
       <c r="B92">
-        <v>8.2461999999999994E-2</v>
+        <v>7.4464000000000002E-2</v>
       </c>
       <c r="C92">
-        <v>2.6699999999999998E-4</v>
+        <v>1.4200000000000001E-4</v>
       </c>
       <c r="D92">
-        <v>0.92146600000000001</v>
+        <v>0.15732399999999999</v>
       </c>
       <c r="E92">
-        <v>1E-4</v>
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="F92">
-        <v>6.9642999999999997E-2</v>
+        <v>7.0093000000000003E-2</v>
       </c>
       <c r="G92">
-        <v>9.9129999999999999E-3</v>
+        <v>9.8359999999999993E-3</v>
       </c>
       <c r="H92">
         <v>256</v>
       </c>
       <c r="I92">
-        <v>1.0735710000000001</v>
+        <v>0.30188100000000001</v>
       </c>
       <c r="J92" t="s">
         <v>7</v>
@@ -4221,28 +4221,28 @@
         <v>67108864</v>
       </c>
       <c r="B93">
-        <v>0.16894000000000001</v>
+        <v>0.15407100000000001</v>
       </c>
       <c r="C93">
-        <v>3.68E-4</v>
+        <v>1.6100000000000001E-3</v>
       </c>
       <c r="D93">
-        <v>1.9069069999999999</v>
+        <v>0.31095899999999999</v>
       </c>
       <c r="E93">
-        <v>5.4900000000000001E-4</v>
+        <v>1.866E-3</v>
       </c>
       <c r="F93">
-        <v>0.138206</v>
+        <v>0.13807700000000001</v>
       </c>
       <c r="G93">
-        <v>1.8464999999999999E-2</v>
+        <v>1.8214999999999999E-2</v>
       </c>
       <c r="H93">
         <v>256</v>
       </c>
       <c r="I93">
-        <v>2.2140529999999998</v>
+        <v>0.60310699999999995</v>
       </c>
       <c r="J93" t="s">
         <v>7</v>
@@ -4253,7 +4253,7 @@
         <v>15</v>
       </c>
       <c r="B94">
-        <v>1.64E-4</v>
+        <v>1.4200000000000001E-4</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>